<commit_message>
Cambios documento word PDD
Se cambiaron los requerimientos funcionales
2. Se agregaron los requisitos
</commit_message>
<xml_diff>
--- a/Document/Historias de usuarios 10-20.xlsx
+++ b/Document/Historias de usuarios 10-20.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\OneDrive\Escritorio\Todo pc\U\U9\Diseño multimedia\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\OneDrive\Escritorio\IZZI-PARKING\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4866B7C5-1141-46AF-951F-2D27DB584505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE0CE4C-7401-45BD-A265-92E5386FDCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4CB1E942-1453-4259-B835-5830CD85585F}"/>
   </bookViews>
@@ -185,7 +185,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +203,13 @@
     <font>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -366,24 +373,123 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -394,149 +500,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -854,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B221892F-3E93-4B11-9A40-4D4A86A9598F}">
   <dimension ref="A5:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48:I50"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,19 +932,19 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="16">
+      <c r="C6" s="47">
         <v>1</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>10</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>4</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -911,11 +955,11 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="17"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="1" t="s">
         <v>28</v>
       </c>
@@ -924,11 +968,11 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="18"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="1" t="s">
         <v>29</v>
       </c>
@@ -937,19 +981,19 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="16">
+      <c r="C9" s="47">
         <v>2</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="5">
-        <v>4</v>
-      </c>
-      <c r="G9" s="5">
+      <c r="F9" s="3">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3">
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -960,11 +1004,11 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="1" t="s">
         <v>31</v>
       </c>
@@ -973,11 +1017,11 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="1" t="s">
         <v>32</v>
       </c>
@@ -986,56 +1030,56 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="40" t="s">
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="5">
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="3">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="6"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="4"/>
     </row>
     <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="7"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="16">
+      <c r="C15" s="47">
         <v>3</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="3">
         <v>7</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="3">
         <v>3</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -1046,11 +1090,11 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="17"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1059,11 +1103,11 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="18"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="1" t="s">
         <v>33</v>
       </c>
@@ -1072,22 +1116,22 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="5">
-        <v>4</v>
-      </c>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="3">
+        <v>4</v>
+      </c>
+      <c r="D18" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="58">
         <v>3</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="58">
         <v>8</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="59" t="s">
         <v>30</v>
       </c>
       <c r="I18" s="1">
@@ -1095,12 +1139,12 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="6"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="1" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="59" t="s">
         <v>35</v>
       </c>
       <c r="I19" s="1">
@@ -1108,12 +1152,12 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="1" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="59" t="s">
         <v>32</v>
       </c>
       <c r="I20" s="1">
@@ -1121,59 +1165,59 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="31" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="5">
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="3">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="6"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="7"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>5</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="5">
-        <v>4</v>
-      </c>
-      <c r="G24" s="5">
+      <c r="F24" s="58">
+        <v>4</v>
+      </c>
+      <c r="G24" s="58">
         <v>7</v>
       </c>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="59" t="s">
         <v>30</v>
       </c>
       <c r="I24" s="1">
@@ -1181,12 +1225,12 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="6"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="1" t="s">
+      <c r="C25" s="4"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="59" t="s">
         <v>36</v>
       </c>
       <c r="I25" s="1">
@@ -1194,12 +1238,12 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="7"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="1" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="59" t="s">
         <v>37</v>
       </c>
       <c r="I26" s="1">
@@ -1207,22 +1251,22 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="16">
+      <c r="C27" s="47">
         <v>6</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="F27" s="5">
-        <v>4</v>
-      </c>
-      <c r="G27" s="5">
+      <c r="F27" s="58">
+        <v>4</v>
+      </c>
+      <c r="G27" s="58">
         <v>5</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="H27" s="59" t="s">
         <v>30</v>
       </c>
       <c r="I27" s="1">
@@ -1230,12 +1274,12 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C28" s="17"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="1" t="s">
+      <c r="C28" s="48"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="59" t="s">
         <v>31</v>
       </c>
       <c r="I28" s="1">
@@ -1243,12 +1287,12 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C29" s="18"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="1" t="s">
+      <c r="C29" s="49"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="59" t="s">
         <v>32</v>
       </c>
       <c r="I29" s="1">
@@ -1256,59 +1300,59 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="40" t="s">
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="5">
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="44"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="6"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="47"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="48"/>
-      <c r="I32" s="7"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="5">
+      <c r="C33" s="3">
         <v>7</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="58">
         <v>5</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="58">
         <v>6</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H33" s="59" t="s">
         <v>30</v>
       </c>
       <c r="I33" s="1">
@@ -1316,12 +1360,12 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="6"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="1" t="s">
+      <c r="C34" s="4"/>
+      <c r="D34" s="70"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="59" t="s">
         <v>31</v>
       </c>
       <c r="I34" s="1">
@@ -1329,12 +1373,12 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C35" s="7"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="1" t="s">
+      <c r="C35" s="5"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="59" t="s">
         <v>32</v>
       </c>
       <c r="I35" s="1">
@@ -1342,19 +1386,19 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C36" s="5">
+      <c r="C36" s="3">
         <v>8</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="28" t="s">
+      <c r="E36" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="3">
         <v>6</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="3">
         <v>6</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -1365,11 +1409,11 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C37" s="6"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
       <c r="H37" s="1" t="s">
         <v>38</v>
       </c>
@@ -1378,11 +1422,11 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="7"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
       <c r="H38" s="1" t="s">
         <v>39</v>
       </c>
@@ -1391,56 +1435,56 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="31" t="s">
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="33"/>
-      <c r="I39" s="5">
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="49"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="35"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="6"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="22"/>
+      <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="39"/>
-      <c r="I41" s="7"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="5">
+      <c r="C42" s="3">
         <v>9</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="8" t="s">
+      <c r="E42" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F42" s="5">
+      <c r="F42" s="3">
         <v>7</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="3">
         <v>3</v>
       </c>
       <c r="H42" s="1" t="s">
@@ -1451,11 +1495,11 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C43" s="6"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
       <c r="H43" s="1" t="s">
         <v>40</v>
       </c>
@@ -1464,11 +1508,11 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C44" s="7"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="10"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
       <c r="H44" s="1" t="s">
         <v>32</v>
       </c>
@@ -1477,19 +1521,19 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C45" s="5">
+      <c r="C45" s="3">
         <v>10</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="3">
         <v>6</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="3">
         <v>3</v>
       </c>
       <c r="H45" s="1" t="s">
@@ -1500,11 +1544,11 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C46" s="6"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="42"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
       <c r="H46" s="1" t="s">
         <v>41</v>
       </c>
@@ -1513,11 +1557,11 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C47" s="7"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
       <c r="H47" s="1" t="s">
         <v>42</v>
       </c>
@@ -1526,50 +1570,50 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C48" s="50" t="s">
+      <c r="C48" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="51"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="51"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="5">
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="3">
         <v>22</v>
       </c>
     </row>
     <row r="49" spans="3:9" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C49" s="53"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="54"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="6"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="4"/>
     </row>
     <row r="50" spans="3:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="56"/>
-      <c r="D50" s="57"/>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="7"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="15"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="5"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C51" s="4">
+      <c r="C51" s="54">
         <v>11</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E51" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F51" s="4">
+      <c r="F51" s="54">
         <v>6</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="54">
         <v>3</v>
       </c>
       <c r="H51" s="1" t="s">
@@ -1580,11 +1624,11 @@
       </c>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C52" s="4"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="11"/>
-      <c r="F52" s="4"/>
-      <c r="G52" s="4"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="55"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="54"/>
       <c r="H52" s="1" t="s">
         <v>41</v>
       </c>
@@ -1593,11 +1637,11 @@
       </c>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C53" s="4"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="11"/>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
+      <c r="C53" s="54"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="54"/>
       <c r="H53" s="1" t="s">
         <v>42</v>
       </c>
@@ -1606,73 +1650,141 @@
       </c>
     </row>
     <row r="54" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
       <c r="I54" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="55" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
     </row>
     <row r="56" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
     </row>
     <row r="57" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
     </row>
     <row r="58" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
     </row>
     <row r="59" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
     </row>
     <row r="60" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
     </row>
     <row r="61" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="G51:G53"/>
+    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="G57:G59"/>
+    <mergeCell ref="G60:G62"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="G45:G47"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="F54:F56"/>
+    <mergeCell ref="F57:F59"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="E57:E59"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="C60:C62"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="D54:D56"/>
+    <mergeCell ref="D57:D59"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="C45:C47"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="G6:G8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="E27:E29"/>
+    <mergeCell ref="F27:F29"/>
+    <mergeCell ref="G27:G29"/>
     <mergeCell ref="I48:I50"/>
     <mergeCell ref="A39:B41"/>
     <mergeCell ref="A30:B32"/>
@@ -1689,74 +1801,6 @@
     <mergeCell ref="I30:I32"/>
     <mergeCell ref="C36:C38"/>
     <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="G36:G38"/>
-    <mergeCell ref="E27:E29"/>
-    <mergeCell ref="F27:F29"/>
-    <mergeCell ref="G27:G29"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="C27:C29"/>
-    <mergeCell ref="D27:D29"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="G6:G8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C60:C62"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="D54:D56"/>
-    <mergeCell ref="D57:D59"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="C45:C47"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="E57:E59"/>
-    <mergeCell ref="E60:E62"/>
-    <mergeCell ref="F45:F47"/>
-    <mergeCell ref="G45:G47"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="F54:F56"/>
-    <mergeCell ref="F57:F59"/>
-    <mergeCell ref="F60:F62"/>
-    <mergeCell ref="G51:G53"/>
-    <mergeCell ref="G54:G56"/>
-    <mergeCell ref="G57:G59"/>
-    <mergeCell ref="G60:G62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>